<commit_message>
Add historical wildfire layers, issue #70
Also correct some point locations.
Fix issue with RMNP not loading.
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Administration-CoDwrWaterDistricts/data/dwr-offices.xlsx
+++ b/workflow/BasinEntities/Administration-CoDwrWaterDistricts/data/dwr-offices.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sam\owf-dev\App-Poudre-Portal\git-repos\owf-app-poudre-dashboard-workflow\workflow\BasinEntities\Administrative-WaterDistricts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sam\owf-dev\InfoMapper-Poudre\git-repos\owf-infomapper-poudre\workflow\BasinEntities\Administration-CoDwrWaterDistricts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -51,7 +51,7 @@
     <t>the information was retrieved from the DWR website (http://water.state.co.us/DivisionsOffices/Div1SPlatteRiverBasin/Pages/Div1SPlatteRB.aspx) and Google Maps.</t>
   </si>
   <si>
-    <t>http://water.state.co.us/DivisionsOffices/Div1SPlatteRiverBasin/Pages/Div1SPlatteRB.aspx</t>
+    <t>https://dwr.colorado.gov/division-offices/division-1-office</t>
   </si>
 </sst>
 </file>
@@ -471,10 +471,7 @@
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Commit initial dashboard files, issue #164
This does NOT include dynamic downloads and workflow results.
</commit_message>
<xml_diff>
--- a/workflow/BasinEntities/Administration-CoDwrWaterDistricts/data/dwr-offices.xlsx
+++ b/workflow/BasinEntities/Administration-CoDwrWaterDistricts/data/dwr-offices.xlsx
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>This workbook contains the list of Colorado Division of Water Resources offices for Division 1.</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="37">
   <si>
     <t>The Data worksheet is converted into a GeoJSON file for use in the Poudre Basin Information portal.</t>
   </si>
@@ -45,13 +42,100 @@
     <t>Latitude</t>
   </si>
   <si>
-    <t>Division 1 Office (Greeley)</t>
-  </si>
-  <si>
     <t>the information was retrieved from the DWR website (http://water.state.co.us/DivisionsOffices/Div1SPlatteRiverBasin/Pages/Div1SPlatteRB.aspx) and Google Maps.</t>
   </si>
   <si>
     <t>https://dwr.colorado.gov/division-offices/division-1-office</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Division 1 Sterling Office</t>
+  </si>
+  <si>
+    <t>Division 1 Main Office (Greeley)</t>
+  </si>
+  <si>
+    <t>Division 2 Main Office (Pueblo)</t>
+  </si>
+  <si>
+    <t>https://dwr.colorado.gov/division-offices/division-2-office</t>
+  </si>
+  <si>
+    <t>Division 2 Colorado Springs Office</t>
+  </si>
+  <si>
+    <t>Division 2 La Junta Office</t>
+  </si>
+  <si>
+    <t>https://dwr.colorado.gov/division-offices/division-3-office</t>
+  </si>
+  <si>
+    <t>Division 3 Main Office (Alamosa)</t>
+  </si>
+  <si>
+    <t>Division 3 Monte Vista Office</t>
+  </si>
+  <si>
+    <t>Division 3 Antonito Office</t>
+  </si>
+  <si>
+    <t>Division 3 Saguache Office</t>
+  </si>
+  <si>
+    <t>https://dwr.colorado.gov/division-offices/division-4-office</t>
+  </si>
+  <si>
+    <t>Division 4 Main Office (Montrose)</t>
+  </si>
+  <si>
+    <t>Division 4 Cedaredge Office</t>
+  </si>
+  <si>
+    <t>https://dwr.colorado.gov/division-offices/division-5-office</t>
+  </si>
+  <si>
+    <t>Division 5 Main Office (Glenwood Springs)</t>
+  </si>
+  <si>
+    <t>Division 5 Upper River Office</t>
+  </si>
+  <si>
+    <t>Division 5 Grand Junction Office</t>
+  </si>
+  <si>
+    <t>https://dwr.colorado.gov/division-offices/division-6-office</t>
+  </si>
+  <si>
+    <t>Division 6 Main Office (Steamboat Springs)</t>
+  </si>
+  <si>
+    <t>Division 6 Craig Office</t>
+  </si>
+  <si>
+    <t>https://dwr.colorado.gov/division-offices/division-7-office</t>
+  </si>
+  <si>
+    <t>Division 7 Main Office (Durango)</t>
+  </si>
+  <si>
+    <t>Division 7 Cortez Office</t>
+  </si>
+  <si>
+    <t>Division 7 Pagosa Springs Office</t>
+  </si>
+  <si>
+    <t>No physical address.</t>
+  </si>
+  <si>
+    <t>This workbook contains the list of Colorado Division of Water Resources offices for all Divisions.</t>
+  </si>
+  <si>
+    <t>Updated 2021-07-20</t>
+  </si>
+  <si>
+    <t>Comment</t>
   </si>
 </sst>
 </file>
@@ -403,22 +487,22 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>44337</v>
+      <c r="A4" s="1" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -428,50 +512,369 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="31.5546875" customWidth="1"/>
-    <col min="2" max="2" width="77.77734375" customWidth="1"/>
-    <col min="3" max="3" width="13.88671875" customWidth="1"/>
-    <col min="4" max="4" width="9.44140625" customWidth="1"/>
+    <col min="1" max="1" width="36.21875" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" customWidth="1"/>
+    <col min="3" max="3" width="77.77734375" customWidth="1"/>
+    <col min="4" max="4" width="13.88671875" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" customWidth="1"/>
+    <col min="6" max="6" width="24.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>-104.77084000000001</v>
+      </c>
+      <c r="E2">
+        <v>40.409419999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>-103.19913</v>
+      </c>
+      <c r="E3">
+        <v>40.634810000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4">
+        <v>-104.61754999999999</v>
+      </c>
+      <c r="E4">
+        <v>38.257370000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5">
+        <v>-104.82989000000001</v>
+      </c>
+      <c r="E5">
+        <v>38.894060000000003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>-103.5427</v>
+      </c>
+      <c r="E6">
+        <v>37.985860000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7">
+        <v>-105.88508</v>
+      </c>
+      <c r="E7">
+        <v>37.475810000000003</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>-106.14794000000001</v>
+      </c>
+      <c r="E8">
+        <v>37.579520000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <v>-106.00913</v>
+      </c>
+      <c r="E9">
+        <v>37.074950000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10">
+        <v>-106.13658</v>
+      </c>
+      <c r="E10">
+        <v>38.08849</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D11">
+        <v>-107.86503999999999</v>
+      </c>
+      <c r="E11">
+        <v>38.447499999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12">
+        <v>-107.93396</v>
+      </c>
+      <c r="E12">
+        <v>38.900869999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>-107.36557000000001</v>
+      </c>
+      <c r="E13">
+        <v>39.563949999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14">
+        <v>5</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>-105.94141</v>
+      </c>
+      <c r="E14">
+        <v>40.085479999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>-108.53892999999999</v>
+      </c>
+      <c r="E15">
+        <v>39.11656</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2">
-        <v>-104.69153</v>
-      </c>
-      <c r="D2">
-        <v>40.423630000000003</v>
+      <c r="C16" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16">
+        <v>-106.82223999999999</v>
+      </c>
+      <c r="E16">
+        <v>40.46622</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>6</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17">
+        <v>-107.54705</v>
+      </c>
+      <c r="E17">
+        <v>40.512740000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>-107.89004</v>
+      </c>
+      <c r="E18">
+        <v>37.271740000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D19">
+        <v>-108.55997000000001</v>
+      </c>
+      <c r="E19">
+        <v>37.347839999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="F20" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C4" r:id="rId2"/>
+    <hyperlink ref="C19" r:id="rId3"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>